<commit_message>
nm commit del lab
</commit_message>
<xml_diff>
--- a/Lab1_Procesos/datos_mediciones lab 1 parte1y2.xlsx
+++ b/Lab1_Procesos/datos_mediciones lab 1 parte1y2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richie\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laboratorio_SO_Ricardo-Paredes\Lab1_Procesos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BE2879-82C8-460C-90F3-FC382F10547A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C367A-65CD-4A32-846B-92044F563FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{801150B8-E90B-492B-B323-396CFAA9DC37}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11835" xr2:uid="{801150B8-E90B-492B-B323-396CFAA9DC37}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Observaciones</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t>Proceso finalizado</t>
+  </si>
+  <si>
+    <t>Terminado</t>
   </si>
 </sst>
 </file>
@@ -221,12 +224,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -238,33 +256,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78B8D407-1D4C-4FF0-AF25-D67EEBEC0239}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:H7"/>
+      <selection activeCell="A11" sqref="A11:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,306 +619,317 @@
     <col min="18" max="18" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="2" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="11"/>
-      <c r="S2" s="5"/>
-    </row>
-    <row r="3" spans="1:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="H2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
         <v>10</v>
       </c>
-      <c r="B3" s="8">
-        <v>1</v>
-      </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="12"/>
-    </row>
-    <row r="4" spans="1:19" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
         <v>20</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12" t="s">
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="12"/>
-    </row>
-    <row r="5" spans="1:19" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
         <v>30</v>
       </c>
-      <c r="B5" s="8">
-        <v>1</v>
-      </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
-        <v>1</v>
-      </c>
-      <c r="E5" s="8">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="s">
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="12"/>
-    </row>
-    <row r="6" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:19" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="1:19" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="I12" s="9"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11">
         <v>0.93990740740740741</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <v>1.3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="10">
         <v>0.2</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4" t="s">
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="I13" s="9"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
         <v>0.9399305555555556</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="10">
         <v>0</v>
       </c>
-      <c r="F14" s="3">
+      <c r="E14" s="10"/>
+      <c r="F14" s="12">
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="10">
         <v>2</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="I14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="I14" s="9"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="11">
         <v>0.93996527777777783</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="10">
         <v>3</v>
       </c>
-      <c r="F15" s="3">
+      <c r="E15" s="10"/>
+      <c r="F15" s="12">
         <v>3.4722222222222224E-4</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="10">
         <v>3</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="4"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="I15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="11">
         <v>0.94003472222222217</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="5">
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="10">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10">
         <v>3.1</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="I16" s="4"/>
+      <c r="I16" s="9"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="11">
         <v>0.93958333333333333</v>
       </c>
-      <c r="F17" t="s">
+      <c r="B17" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="10">
         <v>9.1</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="4"/>
+      <c r="I17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:H7"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="H16:I16"/>
     <mergeCell ref="H17:I17"/>
@@ -909,7 +938,11 @@
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H13:I13"/>
     <mergeCell ref="H14:I14"/>
-    <mergeCell ref="A6:H7"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>